<commit_message>
Se hace el merge de los dos archivos
</commit_message>
<xml_diff>
--- a/scac/BackEnd/resultado_validaciones.xlsx
+++ b/scac/BackEnd/resultado_validaciones.xlsx
@@ -625,7 +625,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CLAUDIA PATRICIA GRAVIER CALDERON</t>
+          <t>CLAUDSD PATRICIA GRAVIER CALDERON</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>VERIFICADO</t>
+          <t>NO VERIFICADO</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
@@ -971,35 +971,17 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>VERIFICADO</t>
+          <t>NO VERIFICADO</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>LIZETH VANESSA PEDREROS ARANGO</t>
-        </is>
-      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">

</xml_diff>